<commit_message>
Cập nhật code sau khi sửa
</commit_message>
<xml_diff>
--- a/output_hoa_don_final.xlsx
+++ b/output_hoa_don_final.xlsx
@@ -514,14 +514,42 @@
           <t>https://tracuuhoadon.fpt.com.vn/search.html</t>
         </is>
       </c>
-      <c r="E2" t="inlineStr"/>
-      <c r="F2" t="inlineStr"/>
-      <c r="G2" t="inlineStr"/>
-      <c r="H2" t="inlineStr"/>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>00068496</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>CÔNG TY CỔ PHẦN BA HUÂN</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>0304244470</t>
+        </is>
+      </c>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>22 Nguyễn Đình Chi, Phường 09, Quận 6, Thành phố Hồ Chí Minh, Việt Nam</t>
+        </is>
+      </c>
       <c r="I2" t="inlineStr"/>
-      <c r="J2" t="inlineStr"/>
-      <c r="K2" t="inlineStr"/>
-      <c r="L2" t="inlineStr"/>
+      <c r="J2" t="inlineStr">
+        <is>
+          <t>Liên Hiệp Hợp Tác Xã Thương Mại TP. Hồ Chí Minh</t>
+        </is>
+      </c>
+      <c r="K2" t="inlineStr">
+        <is>
+          <t>199-205 Nguyễn Thái Học, Phường Phạm Ngũ Lão, Quận 1, Thành phố Hồ Chí Minh, Việt Nam</t>
+        </is>
+      </c>
+      <c r="L2" t="inlineStr">
+        <is>
+          <t>0301175691</t>
+        </is>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
@@ -570,14 +598,46 @@
           <t>https://tracuuhoadon.fpt.com.vn/search.html</t>
         </is>
       </c>
-      <c r="E4" t="inlineStr"/>
-      <c r="F4" t="inlineStr"/>
-      <c r="G4" t="inlineStr"/>
-      <c r="H4" t="inlineStr"/>
-      <c r="I4" t="inlineStr"/>
-      <c r="J4" t="inlineStr"/>
-      <c r="K4" t="inlineStr"/>
-      <c r="L4" t="inlineStr"/>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>00023079</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>CÔNG TY CỔ PHẦN PHÚ TRƯỜNG QUỐC TẾ</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>0304308445</t>
+        </is>
+      </c>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>15A1 Đường Nguyễn Hữu Thọ, Xã Phước Kiển, Huyện Nhà Bè, Thành phố Hồ Chí Minh, Việt Nam</t>
+        </is>
+      </c>
+      <c r="I4" t="inlineStr">
+        <is>
+          <t>0181003527080</t>
+        </is>
+      </c>
+      <c r="J4" t="inlineStr">
+        <is>
+          <t>Liên Hiệp Hợp Tác Xã Thương Mại TP.HCM</t>
+        </is>
+      </c>
+      <c r="K4" t="inlineStr">
+        <is>
+          <t>199-205 Nguyễn Thái Học, Phường Phạm Ngũ Lão, Quận 01, Thành Phố Hồ Chí Minh</t>
+        </is>
+      </c>
+      <c r="L4" t="inlineStr">
+        <is>
+          <t>0301175691</t>
+        </is>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
@@ -598,14 +658,46 @@
           <t>https://www.meinvoice.vn/tra-cuu/</t>
         </is>
       </c>
-      <c r="E5" t="inlineStr"/>
-      <c r="F5" t="inlineStr"/>
-      <c r="G5" t="inlineStr"/>
-      <c r="H5" t="inlineStr"/>
-      <c r="I5" t="inlineStr"/>
-      <c r="J5" t="inlineStr"/>
-      <c r="K5" t="inlineStr"/>
-      <c r="L5" t="inlineStr"/>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>00002426</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>CÔNG TY TNHH CHĂN NUÔI TAFA VIỆT</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>3401142134</t>
+        </is>
+      </c>
+      <c r="H5" t="inlineStr">
+        <is>
+          <t>Thôn 1, Xã Trà Tân, Huyện Đức Linh, Tỉnh Bình Thuận, Việt Nam</t>
+        </is>
+      </c>
+      <c r="I5" t="inlineStr">
+        <is>
+          <t>5400 201 010 928</t>
+        </is>
+      </c>
+      <c r="J5" t="inlineStr">
+        <is>
+          <t>CÔNG TY TNHH MỘT THÀNH VIÊN TMDV SIÊU THỊ CO.OPMART ĐÀ NẴNG</t>
+        </is>
+      </c>
+      <c r="K5" t="inlineStr">
+        <is>
+          <t>478 Điện Biên Phủ, Phường Thanh Khê Đông, Quận Thanh Khê, Thành phố Đà Nẵng, Việt Nam</t>
+        </is>
+      </c>
+      <c r="L5" t="inlineStr">
+        <is>
+          <t>0401281414</t>
+        </is>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
@@ -654,14 +746,46 @@
           <t>https://www.meinvoice.vn/tra-cuu/</t>
         </is>
       </c>
-      <c r="E7" t="inlineStr"/>
-      <c r="F7" t="inlineStr"/>
-      <c r="G7" t="inlineStr"/>
-      <c r="H7" t="inlineStr"/>
-      <c r="I7" t="inlineStr"/>
-      <c r="J7" t="inlineStr"/>
-      <c r="K7" t="inlineStr"/>
-      <c r="L7" t="inlineStr"/>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>00000094</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>CÔNG TY TNHH ĐẦU TƯ - SẢN XUẤT VÀ THƯƠNG MẠI HOÀNG BÁCH</t>
+        </is>
+      </c>
+      <c r="G7" t="inlineStr">
+        <is>
+          <t>0318580994</t>
+        </is>
+      </c>
+      <c r="H7" t="inlineStr">
+        <is>
+          <t>C9/16A31 Bùi Thanh Khiết, khu phố 3, Thị Trấn Tân Túc, Huyện Bình Chánh, Thành phố Hồ Chí Minh, Việt Nam</t>
+        </is>
+      </c>
+      <c r="I7" t="inlineStr">
+        <is>
+          <t>110605110688</t>
+        </is>
+      </c>
+      <c r="J7" t="inlineStr">
+        <is>
+          <t>CHI NHÁNH LIÊN HIỆP HỢP TÁC XÃ THƯƠNG MẠI TP.HỒ CHÍ MINH - CO.OPMART CHU VĂN AN</t>
+        </is>
+      </c>
+      <c r="K7" t="inlineStr">
+        <is>
+          <t>Tầng 1-Tầng 2 Khối A&amp;B Cao ốc Đất Phương Nam 241A Chu Văn An, Phường 12, Quận Bình Thạnh, TP Hồ Chí Minh</t>
+        </is>
+      </c>
+      <c r="L7" t="inlineStr">
+        <is>
+          <t>0301175691-036</t>
+        </is>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
@@ -682,14 +806,42 @@
           <t>https://van.ehoadon.vn/TCHD?MTC=</t>
         </is>
       </c>
-      <c r="E8" t="inlineStr"/>
-      <c r="F8" t="inlineStr"/>
-      <c r="G8" t="inlineStr"/>
-      <c r="H8" t="inlineStr"/>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>00004221</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>CÔNG TY TNHH SẢN XUẤT THƯƠNG MẠI DỊCH VỤ NAM KHẢI PHÚ</t>
+        </is>
+      </c>
+      <c r="G8" t="inlineStr">
+        <is>
+          <t>0312563329</t>
+        </is>
+      </c>
+      <c r="H8" t="inlineStr">
+        <is>
+          <t>81 Cách Mạng Tháng Tám, Phường Bến Thành, Quận 1, Hồ Chí Minh</t>
+        </is>
+      </c>
       <c r="I8" t="inlineStr"/>
-      <c r="J8" t="inlineStr"/>
-      <c r="K8" t="inlineStr"/>
-      <c r="L8" t="inlineStr"/>
+      <c r="J8" t="inlineStr">
+        <is>
+          <t>Chi Nhánh Liên Hiệp Hợp Tác Xã Thương Mại TP.Hồ Chí Minh - Co.opMart Cái Bè</t>
+        </is>
+      </c>
+      <c r="K8" t="inlineStr">
+        <is>
+          <t>Khu 2, Thị trấn Cái Bè, Huyện Cái Bè, Tỉnh Tiền Giang</t>
+        </is>
+      </c>
+      <c r="L8" t="inlineStr">
+        <is>
+          <t>0301175691-068</t>
+        </is>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="n">
@@ -738,14 +890,42 @@
           <t>https://van.ehoadon.vn/TCHD?MTC=</t>
         </is>
       </c>
-      <c r="E10" t="inlineStr"/>
-      <c r="F10" t="inlineStr"/>
-      <c r="G10" t="inlineStr"/>
-      <c r="H10" t="inlineStr"/>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>00004288</t>
+        </is>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>CÔNG TY TNHH SẢN XUẤT THƯƠNG MẠI DỊCH VỤ NAM KHẢI PHÚ</t>
+        </is>
+      </c>
+      <c r="G10" t="inlineStr">
+        <is>
+          <t>0312563329</t>
+        </is>
+      </c>
+      <c r="H10" t="inlineStr">
+        <is>
+          <t>81 Cách Mạng Tháng Tám, Phường Bến Thành, Quận 1, Hồ Chí Minh</t>
+        </is>
+      </c>
       <c r="I10" t="inlineStr"/>
-      <c r="J10" t="inlineStr"/>
-      <c r="K10" t="inlineStr"/>
-      <c r="L10" t="inlineStr"/>
+      <c r="J10" t="inlineStr">
+        <is>
+          <t>Chi Nhánh Liên Hiệp Hợp Tác Xã Thương Mại TP.Hồ Chí Minh - Co.opMart Cái Bè</t>
+        </is>
+      </c>
+      <c r="K10" t="inlineStr">
+        <is>
+          <t>Khu 2, Thị trấn Cái Bè, Huyện Cái Bè, Tỉnh Tiền Giang</t>
+        </is>
+      </c>
+      <c r="L10" t="inlineStr">
+        <is>
+          <t>0301175691-068</t>
+        </is>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>